<commit_message>
Added all criteria and some optimisation
</commit_message>
<xml_diff>
--- a/Gantt Chart.xlsx
+++ b/Gantt Chart.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marko\Desktop\Coding\internalAssesment\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marko\Desktop\cs ia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEBE7A0B-7222-477E-A79C-D006F6D1FEF5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{222865CB-32FF-4AEB-8C9B-0F4C42EFA06F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{37691B4F-8D01-3D41-A1F7-19F7E51539BA}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Week beg 09/02</t>
   </si>
@@ -93,64 +93,22 @@
     <t>Evaluation</t>
   </si>
   <si>
-    <t>Week beg 8/09</t>
-  </si>
-  <si>
-    <t>Week beg 8/02</t>
-  </si>
-  <si>
-    <t>Week beg 8/25</t>
-  </si>
-  <si>
-    <t>Week beg 8/18</t>
-  </si>
-  <si>
-    <t>Week beg 8/11</t>
-  </si>
-  <si>
-    <t>Week beg 8/04</t>
-  </si>
-  <si>
-    <t>Week beg 7/28</t>
-  </si>
-  <si>
-    <t>Week beg 7/21</t>
-  </si>
-  <si>
-    <t>Week beg 7/14</t>
-  </si>
-  <si>
-    <t>Week beg 7/07</t>
-  </si>
-  <si>
-    <t>Week beg 6/30</t>
-  </si>
-  <si>
-    <t>Week beg 6/23</t>
-  </si>
-  <si>
-    <t>Week beg 6/16</t>
-  </si>
-  <si>
-    <t>Week beg 6/09</t>
-  </si>
-  <si>
-    <t>Week beg 6/02</t>
-  </si>
-  <si>
-    <t>Interview Client</t>
-  </si>
-  <si>
-    <t>Information Gathering</t>
-  </si>
-  <si>
-    <t>interface design</t>
-  </si>
-  <si>
-    <t>db design</t>
-  </si>
-  <si>
     <t>functionaility</t>
+  </si>
+  <si>
+    <t>Meeting with Advisor</t>
+  </si>
+  <si>
+    <t>Detailed outline of project and Success criteria</t>
+  </si>
+  <si>
+    <t>Information Gathering, Decide technology</t>
+  </si>
+  <si>
+    <t>user interface , (how to input/output data)</t>
+  </si>
+  <si>
+    <t>functionality of the game</t>
   </si>
 </sst>
 </file>
@@ -172,7 +130,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -185,8 +143,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -194,16 +158,37 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -518,164 +503,486 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2DA75C0-CA90-2B45-937B-24862433A12C}">
-  <dimension ref="A1:AE13"/>
+  <dimension ref="A1:AE14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="16" width="3.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="41.5" customWidth="1"/>
+    <col min="2" max="5" width="3.6640625" customWidth="1"/>
+    <col min="6" max="14" width="3.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="3.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:31" s="1" customFormat="1" ht="84.5" x14ac:dyDescent="0.35">
-      <c r="B1" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="O1" s="1" t="s">
+      <c r="A1" s="2"/>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+      <c r="O2" s="3"/>
+      <c r="P2" s="3"/>
+      <c r="Q2" s="3"/>
+      <c r="R2" s="3"/>
+      <c r="S2" s="3"/>
+      <c r="T2" s="3"/>
+      <c r="U2" s="3"/>
+      <c r="V2" s="3"/>
+      <c r="W2" s="3"/>
+      <c r="X2" s="3"/>
+      <c r="Y2" s="3"/>
+      <c r="Z2" s="3"/>
+      <c r="AA2" s="3"/>
+      <c r="AB2" s="3"/>
+      <c r="AC2" s="3"/>
+      <c r="AD2" s="3"/>
+      <c r="AE2" s="3"/>
+    </row>
+    <row r="3" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A3" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="P1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="Y1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="Z1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="AA1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="AB1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="AC1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="AD1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AE1" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-    </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B3" s="2"/>
-      <c r="E3" s="2"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
+      <c r="O3" s="3"/>
+      <c r="P3" s="3"/>
+      <c r="Q3" s="3"/>
+      <c r="R3" s="3"/>
+      <c r="S3" s="3"/>
+      <c r="T3" s="3"/>
+      <c r="U3" s="3"/>
+      <c r="V3" s="3"/>
+      <c r="W3" s="3"/>
+      <c r="X3" s="3"/>
+      <c r="Y3" s="3"/>
+      <c r="Z3" s="3"/>
+      <c r="AA3" s="3"/>
+      <c r="AB3" s="3"/>
+      <c r="AC3" s="3"/>
+      <c r="AD3" s="3"/>
+      <c r="AE3" s="3"/>
     </row>
     <row r="4" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>36</v>
-      </c>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
+        <v>22</v>
+      </c>
+      <c r="B4" s="3"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
+      <c r="O4" s="3"/>
+      <c r="P4" s="3"/>
+      <c r="Q4" s="3"/>
+      <c r="R4" s="3"/>
+      <c r="S4" s="3"/>
+      <c r="T4" s="3"/>
+      <c r="U4" s="3"/>
+      <c r="V4" s="3"/>
+      <c r="W4" s="3"/>
+      <c r="X4" s="3"/>
+      <c r="Y4" s="3"/>
+      <c r="Z4" s="3"/>
+      <c r="AA4" s="3"/>
+      <c r="AB4" s="3"/>
+      <c r="AC4" s="3"/>
+      <c r="AD4" s="3"/>
+      <c r="AE4" s="3"/>
+    </row>
+    <row r="5" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A5" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
+      <c r="O5" s="3"/>
+      <c r="P5" s="3"/>
+      <c r="Q5" s="3"/>
+      <c r="R5" s="3"/>
+      <c r="S5" s="3"/>
+      <c r="T5" s="3"/>
+      <c r="U5" s="3"/>
+      <c r="V5" s="3"/>
+      <c r="W5" s="3"/>
+      <c r="X5" s="3"/>
+      <c r="Y5" s="3"/>
+      <c r="Z5" s="3"/>
+      <c r="AA5" s="3"/>
+      <c r="AB5" s="3"/>
+      <c r="AC5" s="3"/>
+      <c r="AD5" s="3"/>
+      <c r="AE5" s="3"/>
     </row>
     <row r="6" spans="1:31" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+      <c r="O6" s="3"/>
+      <c r="P6" s="3"/>
+      <c r="Q6" s="3"/>
+      <c r="R6" s="3"/>
+      <c r="S6" s="3"/>
+      <c r="T6" s="3"/>
+      <c r="U6" s="3"/>
+      <c r="V6" s="3"/>
+      <c r="W6" s="3"/>
+      <c r="X6" s="3"/>
+      <c r="Y6" s="3"/>
+      <c r="Z6" s="3"/>
+      <c r="AA6" s="3"/>
+      <c r="AB6" s="3"/>
+      <c r="AC6" s="3"/>
+      <c r="AD6" s="3"/>
+      <c r="AE6" s="3"/>
+    </row>
+    <row r="7" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A7" s="3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>37</v>
-      </c>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="3"/>
+      <c r="O7" s="3"/>
+      <c r="P7" s="3"/>
+      <c r="Q7" s="3"/>
+      <c r="R7" s="3"/>
+      <c r="S7" s="3"/>
+      <c r="T7" s="3"/>
+      <c r="U7" s="3"/>
+      <c r="V7" s="3"/>
+      <c r="W7" s="3"/>
+      <c r="X7" s="3"/>
+      <c r="Y7" s="3"/>
+      <c r="Z7" s="3"/>
+      <c r="AA7" s="3"/>
+      <c r="AB7" s="3"/>
+      <c r="AC7" s="3"/>
+      <c r="AD7" s="3"/>
+      <c r="AE7" s="3"/>
     </row>
     <row r="8" spans="1:31" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>38</v>
-      </c>
+      <c r="A8" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3"/>
+      <c r="M8" s="3"/>
+      <c r="N8" s="3"/>
+      <c r="O8" s="3"/>
+      <c r="P8" s="3"/>
+      <c r="Q8" s="3"/>
+      <c r="R8" s="3"/>
+      <c r="S8" s="3"/>
+      <c r="T8" s="3"/>
+      <c r="U8" s="3"/>
+      <c r="V8" s="3"/>
+      <c r="W8" s="3"/>
+      <c r="X8" s="3"/>
+      <c r="Y8" s="3"/>
+      <c r="Z8" s="3"/>
+      <c r="AA8" s="3"/>
+      <c r="AB8" s="3"/>
+      <c r="AC8" s="3"/>
+      <c r="AD8" s="3"/>
+      <c r="AE8" s="3"/>
     </row>
     <row r="9" spans="1:31" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>39</v>
-      </c>
+      <c r="A9" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
+      <c r="M9" s="3"/>
+      <c r="N9" s="3"/>
+      <c r="O9" s="3"/>
+      <c r="P9" s="3"/>
+      <c r="Q9" s="3"/>
+      <c r="R9" s="3"/>
+      <c r="S9" s="3"/>
+      <c r="T9" s="3"/>
+      <c r="U9" s="3"/>
+      <c r="V9" s="3"/>
+      <c r="W9" s="3"/>
+      <c r="X9" s="3"/>
+      <c r="Y9" s="3"/>
+      <c r="Z9" s="3"/>
+      <c r="AA9" s="3"/>
+      <c r="AB9" s="3"/>
+      <c r="AC9" s="3"/>
+      <c r="AD9" s="3"/>
+      <c r="AE9" s="3"/>
+    </row>
+    <row r="10" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A10" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+      <c r="L10" s="3"/>
+      <c r="M10" s="3"/>
+      <c r="N10" s="3"/>
+      <c r="O10" s="3"/>
+      <c r="P10" s="3"/>
+      <c r="Q10" s="3"/>
+      <c r="R10" s="3"/>
+      <c r="S10" s="3"/>
+      <c r="T10" s="3"/>
+      <c r="U10" s="3"/>
+      <c r="V10" s="3"/>
+      <c r="W10" s="3"/>
+      <c r="X10" s="3"/>
+      <c r="Y10" s="3"/>
+      <c r="Z10" s="3"/>
+      <c r="AA10" s="3"/>
+      <c r="AB10" s="3"/>
+      <c r="AC10" s="3"/>
+      <c r="AD10" s="3"/>
+      <c r="AE10" s="3"/>
     </row>
     <row r="11" spans="1:31" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
+      <c r="A11" s="3"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+      <c r="L11" s="3"/>
+      <c r="M11" s="3"/>
+      <c r="N11" s="3"/>
+      <c r="O11" s="3"/>
+      <c r="P11" s="3"/>
+      <c r="Q11" s="3"/>
+      <c r="R11" s="3"/>
+      <c r="S11" s="3"/>
+      <c r="T11" s="3"/>
+      <c r="U11" s="3"/>
+      <c r="V11" s="3"/>
+      <c r="W11" s="3"/>
+      <c r="X11" s="3"/>
+      <c r="Y11" s="3"/>
+      <c r="Z11" s="3"/>
+      <c r="AA11" s="3"/>
+      <c r="AB11" s="3"/>
+      <c r="AC11" s="3"/>
+      <c r="AD11" s="3"/>
+      <c r="AE11" s="3"/>
+    </row>
+    <row r="12" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A12" s="3" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="12" spans="1:31" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="3"/>
+      <c r="M12" s="3"/>
+      <c r="N12" s="3"/>
+      <c r="O12" s="3"/>
+      <c r="P12" s="3"/>
+      <c r="Q12" s="3"/>
+      <c r="R12" s="3"/>
+      <c r="S12" s="3"/>
+      <c r="T12" s="3"/>
+      <c r="U12" s="3"/>
+      <c r="V12" s="3"/>
+      <c r="W12" s="3"/>
+      <c r="X12" s="3"/>
+      <c r="Y12" s="3"/>
+      <c r="Z12" s="3"/>
+      <c r="AA12" s="3"/>
+      <c r="AB12" s="3"/>
+      <c r="AC12" s="3"/>
+      <c r="AD12" s="3"/>
+      <c r="AE12" s="3"/>
+    </row>
+    <row r="13" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A13" s="3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="13" spans="1:31" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="3"/>
+      <c r="L13" s="3"/>
+      <c r="M13" s="3"/>
+      <c r="N13" s="3"/>
+      <c r="O13" s="3"/>
+      <c r="P13" s="3"/>
+      <c r="Q13" s="3"/>
+      <c r="R13" s="3"/>
+      <c r="S13" s="3"/>
+      <c r="T13" s="3"/>
+      <c r="U13" s="3"/>
+      <c r="V13" s="3"/>
+      <c r="W13" s="3"/>
+      <c r="X13" s="3"/>
+      <c r="Y13" s="3"/>
+      <c r="Z13" s="3"/>
+      <c r="AA13" s="3"/>
+      <c r="AB13" s="3"/>
+      <c r="AC13" s="3"/>
+      <c r="AD13" s="3"/>
+      <c r="AE13" s="3"/>
+    </row>
+    <row r="14" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A14" s="3" t="s">
         <v>19</v>
       </c>
     </row>

</xml_diff>